<commit_message>
first draft linkml schema
</commit_message>
<xml_diff>
--- a/nwb-schema-linkml/project/excel/nwb_schema_language.xlsx
+++ b/nwb-schema-linkml/project/excel/nwb_schema_language.xlsx
@@ -7,9 +7,16 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Namespace" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Namespaces" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="NamespacesCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Schema" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Group" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Attribute" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Link" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Dataset" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ReferenceDtype" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="CompoundDtype" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="AnyType" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +433,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>doc</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -436,7 +443,32 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>full_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>contact</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>schema</t>
         </is>
       </c>
     </row>
@@ -445,68 +477,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -523,11 +512,398 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>namespaces</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>namespace</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>doc</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>neurodata_types</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neurodata_type_def</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neurodata_type_inc</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>default_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>doc</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>linkable</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>attributes</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>datasets</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>groups</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>links</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dims</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>shape</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>default_value</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>doc</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dtype</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>doc</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>target_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neurodata_type_def</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neurodata_type_inc</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>default_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dims</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>shape</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>default_value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>doc</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>linkable</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>attributes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dtype</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>target_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>reftype</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ref,reference,object,region"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>doc</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dtype</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"float,float32,double,float64,long,int64,int,int32,int16,short,int8,uint,uint32,uint16,uint8,uint64,numeric,text,utf,utf8,utf-8,ascii,bool,isodatetime"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>